<commit_message>
API comp: Improve formatting; apply Darlene feedback
</commit_message>
<xml_diff>
--- a/doc/PortageAPIComparison.xlsx
+++ b/doc/PortageAPIComparison.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
   <si>
     <t>Task</t>
   </si>
@@ -187,9 +187,6 @@
     <t>Cleaning up utf8 input</t>
   </si>
   <si>
-    <t>Script clean-utf8-text.pl now standardizes how to clean utf-8 input, both for training corpora (tmx-prepro) and in PortageLive (proprocess_plugin).</t>
-  </si>
-  <si>
     <t>Clean up code exists in preprocess_plugin and tmx-prepro, but not fully consistent.</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>translateTMXCE_Status() or translateSDLXLIFFCE_ Status()</t>
+  </si>
+  <si>
+    <t>Script clean-utf8-text.pl now standardizes how to clean utf-8 input, both for training corpora (tmx-prepro) and in PortageLive (preprocess_plugin).</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -538,76 +538,86 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,454 +935,528 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="22"/>
       <c r="B1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="19" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C28" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="D28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B29" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="D29" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="B31" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>29</v>
-      </c>
+      <c r="C31" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" orientation="landscape" verticalDpi="0" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="21" max="16383" man="1"/>
+  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
+  <rowBreaks count="3" manualBreakCount="3">
+    <brk id="9" max="16383" man="1"/>
+    <brk id="20" max="16383" man="1"/>
+    <brk id="27" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
PortageAPIComparison: add framework features section; review and reformat the whole thing
</commit_message>
<xml_diff>
--- a/doc/PortageAPIComparison.xlsx
+++ b/doc/PortageAPIComparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="30" windowWidth="17220" windowHeight="8475"/>
+    <workbookView xWindow="192" yWindow="36" windowWidth="13968" windowHeight="8472"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="127">
   <si>
     <t>Task</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>Translate one sentence or paragraph</t>
-  </si>
-  <si>
-    <t>same as 2.2</t>
-  </si>
-  <si>
-    <t>Loop over the above procedure, 10 sentences/paragraphs at a time.</t>
   </si>
   <si>
     <t>translateTMXCE()</t>
@@ -94,9 +88,6 @@
     <t>same as 3.0, calling getTranslation2() instead of translate().</t>
   </si>
   <si>
-    <t>The output of grouped queries is not well aligned to the input, so loop over getTranslation2() one sentence at at time.</t>
-  </si>
-  <si>
     <t>loop over getTranslation2() one sentence at at time (expensive overhead: upgrade to a more recent version if speed is an issue).</t>
   </si>
   <si>
@@ -139,9 +130,6 @@
     <t>WSDL Copyright is 2012 and translateSDLXLIFFCE() does not exist</t>
   </si>
   <si>
-    <t>same as 2.0</t>
-  </si>
-  <si>
     <t>translateTMXCE_Status()</t>
   </si>
   <si>
@@ -181,21 +169,12 @@
     <t>Script fix-slashes.pl now used by default in preprocess_plugin.</t>
   </si>
   <si>
-    <t>Separating words joined with slashes (e.g., "inside/outside" -&gt; "inside / outside") so they get translated properly.</t>
-  </si>
-  <si>
-    <t>Cleaning up utf8 input</t>
-  </si>
-  <si>
     <t>Clean up code exists in preprocess_plugin and tmx-prepro, but not fully consistent.</t>
   </si>
   <si>
     <t>Optionally (but not by default), predecode_plugin uses mark-english-number.pl to perform rule-based translation of numbers from English into French only.</t>
   </si>
   <si>
-    <t>Translating fixed terms with constant strings using hard rules</t>
-  </si>
-  <si>
     <t>PortageII 2.1, 2.0, 1.0</t>
   </si>
   <si>
@@ -209,19 +188,6 @@
   </si>
   <si>
     <t>postprocess_plugin has sample code for making some hyphens non-breaking; not enabled by default because encoding is not normalized and depends on the final document file format.</t>
-  </si>
-  <si>
-    <t>Handling numbers between French and English</t>
-  </si>
-  <si>
-    <t>Inserting non-breaking spaces in French output</t>
-  </si>
-  <si>
-    <t>Inserting non-breaking hyphens</t>
-  </si>
-  <si>
-    <t>Use the *FixedTerms API methods to set the rules, which are applied by predecode_plugin;
-Warning: this is not for your whole terminology database, only for absolutely unambiguous terms.</t>
   </si>
   <si>
     <t>Script fix-slashes available in preprocess_plugin; not enabled by default.</t>
@@ -262,6 +228,185 @@
   </si>
   <si>
     <t>Script clean-utf8-text.pl now standardizes how to clean utf-8 input, both for training corpora (tmx-prepro) and in PortageLive (preprocess_plugin).</t>
+  </si>
+  <si>
+    <t>PortageII 3.0 framework</t>
+  </si>
+  <si>
+    <t>PortageII 1.0 framework</t>
+  </si>
+  <si>
+    <t>Need to retrain when upgrading from a previous version?</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII framework features and recommendations from PortageII 1.0 to PortageII 3.0</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>Use of Generic LM (MIXLM_ PRETRAINED_TGT_LMS)</t>
+  </si>
+  <si>
+    <t>Use of Generic TM (MIXTM_PRETRAINED_TMS)</t>
+  </si>
+  <si>
+    <t>Coarse LMs</t>
+  </si>
+  <si>
+    <t>Enable Coarse LMs with 200 and 800 classes (this new features is enabled by default)</t>
+  </si>
+  <si>
+    <t>PortageII 2.2, 2.1 and 2.0 framework</t>
+  </si>
+  <si>
+    <t>BiLM</t>
+  </si>
+  <si>
+    <t>Sparse features (DHDM)</t>
+  </si>
+  <si>
+    <t>HLDM</t>
+  </si>
+  <si>
+    <t>This new feature can sometimes improve system quality but is often not worth it; not enabled by default.</t>
+  </si>
+  <si>
+    <t>Transfer tags from source to target</t>
+  </si>
+  <si>
+    <t>All translate*() methods accept the xtags parameter. Set it to true to transfer tags found in the source text into the target language output.</t>
+  </si>
+  <si>
+    <t>Only supported for TMX and sdlxliff files</t>
+  </si>
+  <si>
+    <t>Set xtags parameter to getTranslation*() or translate*CE()</t>
+  </si>
+  <si>
+    <t>Enable confidence estimation</t>
+  </si>
+  <si>
+    <t>Models must be trained with CE; set useCE parameter to any translate*() method to get confidence estimates with your translations. In TMX and sdlxliff files, the CE score is in a proper field. With translate() or translatePlainText(), it is at the beginning of each line, but the output is only usable if you use nl="s".</t>
+  </si>
+  <si>
+    <t>All *CE() methods compute confidence estimates for models trained with CE. getTranslationCE() and translatePlainTextCE(), output only usable with nl="s".</t>
+  </si>
+  <si>
+    <t>same as 2.2, but not available for plain text files.</t>
+  </si>
+  <si>
+    <t>same as 2.1</t>
+  </si>
+  <si>
+    <t>We now have a specialized pipeline for handling hashtags and tweets from Arabic into English. Ask us if you'd like to enable this for your system and language pair.</t>
+  </si>
+  <si>
+    <t>Clean up utf8 input</t>
+  </si>
+  <si>
+    <t>Separate words joined with slashes (e.g., "inside/outside" -&gt; "inside / outside") so they get translated properly.</t>
+  </si>
+  <si>
+    <t>Handle numbers between French and English</t>
+  </si>
+  <si>
+    <t>Insert non-breaking spaces in French output</t>
+  </si>
+  <si>
+    <t>Insert non-breaking hyphens</t>
+  </si>
+  <si>
+    <t>Translate hashtags in Tweets</t>
+  </si>
+  <si>
+    <t>Translate fixed terms using hard rules</t>
+  </si>
+  <si>
+    <t>Yes.
+PortageII 3.0 includes important new features and many updates to the recommended training parameters: retrain all models from previous versions.</t>
+  </si>
+  <si>
+    <t>Yes.
+This was a major update to the core MT engine, old models should be retrained.</t>
+  </si>
+  <si>
+    <t>No. PortageII 1.0, 2.0, 2.1 and 2.2 models are all compatible. Exceptions: 
+ - a manual step is required to enable fixed terms for models trained before 2.2.
+- the soap-translate.sh file in PortageLive changed between 2.0 and 2.1.</t>
+  </si>
+  <si>
+    <t>optional but recommended</t>
+  </si>
+  <si>
+    <t>The new sparse features, including the discriminitive reordering model, significantly improve translation quality and should always be used.</t>
+  </si>
+  <si>
+    <t>Significance Pruning</t>
+  </si>
+  <si>
+    <t>Use the *FixedTerms API methods to set the rules, which are applied by predecode_plugin;
+Warning: this is not for your whole terminology database, only for absolutely unambiguous terms.
+The fixed-terms functionality was instroducted with PortageII 2.2, but its use is not generally recommended: use only to address specific and problematic errors your trained system makes.</t>
+  </si>
+  <si>
+    <t>The output of grouped queries is not well aligned to the input, so loop over getTranslation2() one sentence or paragraph at time.</t>
+  </si>
+  <si>
+    <t>same as 3.0, calling getTranslation2() instead of translate().
+The explicit control of the semantics of newlines in genTranslation() and getTranslation2() was introduced in 2.1 to facilitate the optimized translation of mini batches of sentences.</t>
+  </si>
+  <si>
+    <t>Loop over the above procedure, 10 sentences or paragraphs at a time. Avoid submitting sentences one at a time if you can, to amortize the fixed overhead over larger blocks instead.</t>
+  </si>
+  <si>
+    <t>This process reduces the size of your phrase tables.
+Only use it for very large, low quality corpora, with 10s of millions or sentence pairs or more.</t>
+  </si>
+  <si>
+    <t>This  baseline reordering model is always required, and should always be used, preferably in combination with the new, sparse one.</t>
+  </si>
+  <si>
+    <t>Source-aware truecasing</t>
+  </si>
+  <si>
+    <t>Use source-aware truecasing whenever possible, i.e., as long as both your source and target language have the concept of case. This feature is automatically disabled for Chinese and Arabic.</t>
+  </si>
+  <si>
+    <t>Tuning with Batch Lattice MIRA</t>
+  </si>
+  <si>
+    <t>Introduced in 1.0, this powerful reordering model is always required.</t>
+  </si>
+  <si>
+    <t>Introduced in 1.0, this state-of-the-art tuning algorithm is always recommended and is the default.</t>
+  </si>
+  <si>
+    <t>Using IBM4 alignments</t>
+  </si>
+  <si>
+    <t>We now recommend systematically using IBM4 alignments, along with the usual IBM2 and HMM3 ones. This produces the most robust and reliable phrase tables.</t>
+  </si>
+  <si>
+    <t>Use this model with your in-domain data to significantly increase the system's vocabulary up front, and potentially improve the quality of all your En&lt;-&gt;Fr models.</t>
+  </si>
+  <si>
+    <t>We now recommend systematically using the Generic LM for all systems between French and English. It cannot introduce out-of-domain terminology, it can only help use your in-domain data better.</t>
+  </si>
+  <si>
+    <t>same as 3.0</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII API from PortageII 1.0 to PortageII 3.0 (p. 2)</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII plugin architecture from PortageII 1.0 to PortageII 3.0 (p. 2)</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII framework features and recommendations from PortageII 1.0 to PortageII 3.0 (p. 2)</t>
+  </si>
+  <si>
+    <t>same as 2.2</t>
   </si>
 </sst>
 </file>
@@ -293,7 +438,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -525,11 +670,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -617,6 +860,81 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -920,24 +1238,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="23.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="23.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -969,32 +1287,32 @@
         <v>2</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>7</v>
@@ -1014,10 +1332,10 @@
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>4</v>
@@ -1037,426 +1355,812 @@
         <v>10</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="45"/>
+      <c r="E7" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="44"/>
+    </row>
+    <row r="8" spans="1:6" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="45"/>
+      <c r="E8" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="44"/>
+    </row>
+    <row r="9" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="D9" s="54"/>
+      <c r="E9" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="55"/>
+    </row>
+    <row r="10" spans="1:6" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="22"/>
+      <c r="B11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="22"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="D15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="15" t="s">
+      <c r="E15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="36" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="C20" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>4</v>
-      </c>
+      <c r="C22" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="22"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="C27" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C28" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>70</v>
-      </c>
       <c r="D29" s="15" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>4</v>
+    <row r="30" spans="1:6" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>55</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>29</v>
-      </c>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="22"/>
+      <c r="B31" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
     </row>
+    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="22"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="22"/>
+      <c r="B40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="22"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="52"/>
+    </row>
+    <row r="43" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="48"/>
+      <c r="E43" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" s="50"/>
+    </row>
+    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" s="42"/>
+    </row>
+    <row r="45" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" s="42"/>
+    </row>
+    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="42"/>
+    </row>
+    <row r="47" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="42"/>
+    </row>
+    <row r="48" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" s="42"/>
+    </row>
+    <row r="49" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="47"/>
+    </row>
+    <row r="50" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="40"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="22"/>
+      <c r="B51" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="22"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" s="52"/>
+    </row>
+    <row r="54" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D54" s="41"/>
+      <c r="E54" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="F54" s="42"/>
+    </row>
+    <row r="55" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="47"/>
+    </row>
+    <row r="56" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="40"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="22"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="22"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="22"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="22"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="22"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="22"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="6"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <mergeCells count="28">
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+  </mergeCells>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
-  <rowBreaks count="3" manualBreakCount="3">
-    <brk id="9" max="16383" man="1"/>
-    <brk id="20" max="16383" man="1"/>
-    <brk id="27" max="16383" man="1"/>
+  <rowBreaks count="5" manualBreakCount="5">
+    <brk id="10" max="16383" man="1"/>
+    <brk id="23" max="16383" man="1"/>
+    <brk id="30" max="16383" man="1"/>
+    <brk id="39" max="16383" man="1"/>
+    <brk id="50" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -1467,7 +2171,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1479,7 +2183,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working on PortageAPIComparison.xlsx for PortageII 4.0
</commit_message>
<xml_diff>
--- a/doc/PortageAPIComparison.xlsx
+++ b/doc/PortageAPIComparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="36" windowWidth="13968" windowHeight="8472"/>
+    <workbookView xWindow="195" yWindow="30" windowWidth="13965" windowHeight="8475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="130">
   <si>
     <t>Task</t>
-  </si>
-  <si>
-    <t>PortageII 3.0 API</t>
   </si>
   <si>
     <t>PortageII 2.0 API</t>
@@ -139,27 +136,6 @@
     <t>getVersion() exists and returns "PortageII-3.0"; WSDL says PortageII 3.0 (2016)</t>
   </si>
   <si>
-    <t>updateFixedTerms()</t>
-  </si>
-  <si>
-    <t>Upload the fixed terms database for a model</t>
-  </si>
-  <si>
-    <t>Get the fixed terms database for a model</t>
-  </si>
-  <si>
-    <t>Erase the fixed terms database for a model</t>
-  </si>
-  <si>
-    <t>getFixedTerms()</t>
-  </si>
-  <si>
-    <t>removeFixedTerms()</t>
-  </si>
-  <si>
-    <t>PortageII 3.0</t>
-  </si>
-  <si>
     <t>PortageLive pipeline</t>
   </si>
   <si>
@@ -218,9 +194,6 @@
     <t>Evolution of the PortageII API from PortageII 1.0 to PortageII 3.0</t>
   </si>
   <si>
-    <t>Evolution of the PortageII plugin architecture from PortageII 1.0 to PortageII 3.0</t>
-  </si>
-  <si>
     <t>translateTMXCE_Status() or translateSDLXLIFFCE_ Status() or translatePlain TextCE_Status()</t>
   </si>
   <si>
@@ -230,18 +203,12 @@
     <t>Script clean-utf8-text.pl now standardizes how to clean utf-8 input, both for training corpora (tmx-prepro) and in PortageLive (preprocess_plugin).</t>
   </si>
   <si>
-    <t>PortageII 3.0 framework</t>
-  </si>
-  <si>
     <t>PortageII 1.0 framework</t>
   </si>
   <si>
     <t>Need to retrain when upgrading from a previous version?</t>
   </si>
   <si>
-    <t>Evolution of the PortageII framework features and recommendations from PortageII 1.0 to PortageII 3.0</t>
-  </si>
-  <si>
     <t>optional</t>
   </si>
   <si>
@@ -284,9 +251,6 @@
     <t>Set xtags parameter to getTranslation*() or translate*CE()</t>
   </si>
   <si>
-    <t>Enable confidence estimation</t>
-  </si>
-  <si>
     <t>Models must be trained with CE; set useCE parameter to any translate*() method to get confidence estimates with your translations. In TMX and sdlxliff files, the CE score is in a proper field. With translate() or translatePlainText(), it is at the beginning of each line, but the output is only usable if you use nl="s".</t>
   </si>
   <si>
@@ -321,10 +285,6 @@
   </si>
   <si>
     <t>Translate fixed terms using hard rules</t>
-  </si>
-  <si>
-    <t>Yes.
-PortageII 3.0 includes important new features and many updates to the recommended training parameters: retrain all models from previous versions.</t>
   </si>
   <si>
     <t>Yes.
@@ -400,13 +360,64 @@
     <t>Evolution of the PortageII API from PortageII 1.0 to PortageII 3.0 (p. 2)</t>
   </si>
   <si>
-    <t>Evolution of the PortageII plugin architecture from PortageII 1.0 to PortageII 3.0 (p. 2)</t>
-  </si>
-  <si>
-    <t>Evolution of the PortageII framework features and recommendations from PortageII 1.0 to PortageII 3.0 (p. 2)</t>
-  </si>
-  <si>
     <t>same as 2.2</t>
+  </si>
+  <si>
+    <t>PortageII 3.0/4.0 API</t>
+  </si>
+  <si>
+    <t>3.0: getAllContexts(verbose)
+4.0: getAllContexts(verbose, json)</t>
+  </si>
+  <si>
+    <t>Enable confidence estimation (slow)</t>
+  </si>
+  <si>
+    <t>Upload / get / erase the fixed terms database for a model</t>
+  </si>
+  <si>
+    <t>updateFixedTerms() / getFixedTerms() / removeFixedTerms()</t>
+  </si>
+  <si>
+    <t>Add a sentence pair to an incremental document model</t>
+  </si>
+  <si>
+    <t>Get the status on incremental document model training</t>
+  </si>
+  <si>
+    <t>4.0: incrAddSentence()</t>
+  </si>
+  <si>
+    <t>4.0: incrStatus()</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII plugin architecture from PortageII 1.0 to PortageII 4.0 (p. 2)</t>
+  </si>
+  <si>
+    <t>PortageII 3.0 and 4.0</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII plugin architecture from PortageII 1.0 to PortageII 4.0</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII framework features and recommendations from PortageII 1.0 to PortageII 4.0</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII framework features and recommendations from PortageII 1.0 to PortageII 4.0 (p. 2)</t>
+  </si>
+  <si>
+    <t>PortageII 3.0 and 4.0 framework</t>
+  </si>
+  <si>
+    <t>3.0: Yes. 3.0 includes important new features and many updates to the recommended training parameters: retrain all models from previous versions.
+4.0: retraining is required to train or fine tune your own NNJM, and to enable incremental document adaptation.</t>
+  </si>
+  <si>
+    <t>NNJM</t>
+  </si>
+  <si>
+    <t>3.0: pre-trained NNJMs available with the generic models for fr-&gt;en and en-&gt;fr.
+4.0: fine-tune the generic NNJM or train your own for best hybrid neural-statistical MT results.</t>
   </si>
 </sst>
 </file>
@@ -772,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -886,56 +897,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1238,24 +1282,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" style="1" customWidth="1"/>
-    <col min="3" max="5" width="23.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="23.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1275,160 +1319,160 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>2</v>
-      </c>
       <c r="F3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="44"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="51"/>
     </row>
     <row r="8" spans="1:6" ht="138" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" s="44"/>
+        <v>46</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="52"/>
+      <c r="E8" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="54"/>
       <c r="E9" s="53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="55"/>
     </row>
     <row r="10" spans="1:6" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1436,207 +1480,207 @@
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>2</v>
-      </c>
       <c r="F13" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>26</v>
+      <c r="D14" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1644,10 +1688,10 @@
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="4" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1664,95 +1708,95 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>46</v>
+        <v>122</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
     </row>
     <row r="27" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B29" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>57</v>
-      </c>
       <c r="D29" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1760,97 +1804,97 @@
       <c r="E32" s="5"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>46</v>
+        <v>122</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="4" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1858,231 +1902,239 @@
       <c r="E41" s="5"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="46"/>
+    </row>
+    <row r="43" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="47"/>
+      <c r="E43" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="49"/>
+    </row>
+    <row r="44" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51" t="s">
+      <c r="B44" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="44"/>
+    </row>
+    <row r="45" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="44"/>
+    </row>
+    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="44"/>
+    </row>
+    <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="44"/>
+    </row>
+    <row r="48" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" s="44"/>
+    </row>
+    <row r="49" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="F42" s="52"/>
-    </row>
-    <row r="43" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C43" s="48" t="s">
+      <c r="B49" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="D43" s="48"/>
-      <c r="E43" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="F43" s="50"/>
-    </row>
-    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="42"/>
-    </row>
-    <row r="45" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B45" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" s="42"/>
-    </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" s="42"/>
-    </row>
-    <row r="47" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="C47" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="42"/>
-    </row>
-    <row r="48" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B48" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C48" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="F48" s="42"/>
-    </row>
-    <row r="49" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="C49" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="47"/>
-    </row>
-    <row r="50" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="B50" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="C50" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="F50" s="40"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D49" s="63"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="64"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="22"/>
+      <c r="B50" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22"/>
-      <c r="B51" s="4" t="s">
-        <v>125</v>
-      </c>
+      <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="22"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="27" t="s">
+    <row r="52" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C53" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="F53" s="52"/>
-    </row>
-    <row r="54" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B52" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="F52" s="46"/>
+    </row>
+    <row r="53" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" s="61"/>
+      <c r="E53" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="62"/>
+    </row>
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="C54" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="F54" s="42"/>
-    </row>
-    <row r="55" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="B55" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="47"/>
-    </row>
-    <row r="56" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="40"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="22"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="6"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="B54" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="44"/>
+    </row>
+    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A55" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="65"/>
+      <c r="E55" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="F55" s="66"/>
+    </row>
+    <row r="56" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="56"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="57"/>
+    </row>
+    <row r="57" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="58"/>
+      <c r="E57" s="58"/>
+      <c r="F57" s="59"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="22"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2090,7 +2142,7 @@
       <c r="E58" s="5"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2098,7 +2150,7 @@
       <c r="E59" s="5"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="22"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2106,7 +2158,7 @@
       <c r="E60" s="5"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -2114,7 +2166,7 @@
       <c r="E61" s="5"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="22"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -2122,8 +2174,36 @@
       <c r="E62" s="5"/>
       <c r="F62" s="6"/>
     </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="30">
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C47:F47"/>
@@ -2134,24 +2214,6 @@
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -2160,7 +2222,7 @@
     <brk id="23" max="16383" man="1"/>
     <brk id="30" max="16383" man="1"/>
     <brk id="39" max="16383" man="1"/>
-    <brk id="50" max="16383" man="1"/>
+    <brk id="49" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -2171,7 +2233,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2183,7 +2245,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
API comparison draft shared with SL, DS, MT today
</commit_message>
<xml_diff>
--- a/doc/PortageAPIComparison.xlsx
+++ b/doc/PortageAPIComparison.xlsx
@@ -133,9 +133,6 @@
     <t>Preload models for a given system so it can run faster</t>
   </si>
   <si>
-    <t>getVersion() exists and returns "PortageII-3.0"; WSDL says PortageII 3.0 (2016)</t>
-  </si>
-  <si>
     <t>PortageLive pipeline</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
   <si>
     <t>As a result of significant improvements in the default PortageLive plugins with PortageII 3.0, you should review all customized plugins you use in your systems and determine if you can use the new default ones instead.
 The plugin architecture continues to allow ad hoc scripts, but most common problems we're aware of are now handled by default.</t>
-  </si>
-  <si>
-    <t>Evolution of the PortageII API from PortageII 1.0 to PortageII 3.0</t>
   </si>
   <si>
     <t>translateTMXCE_Status() or translateSDLXLIFFCE_ Status() or translatePlain TextCE_Status()</t>
@@ -357,9 +351,6 @@
     <t>same as 3.0</t>
   </si>
   <si>
-    <t>Evolution of the PortageII API from PortageII 1.0 to PortageII 3.0 (p. 2)</t>
-  </si>
-  <si>
     <t>same as 2.2</t>
   </si>
   <si>
@@ -385,12 +376,6 @@
     <t>Get the status on incremental document model training</t>
   </si>
   <si>
-    <t>4.0: incrAddSentence()</t>
-  </si>
-  <si>
-    <t>4.0: incrStatus()</t>
-  </si>
-  <si>
     <t>Evolution of the PortageII plugin architecture from PortageII 1.0 to PortageII 4.0 (p. 2)</t>
   </si>
   <si>
@@ -418,6 +403,24 @@
   <si>
     <t>3.0: pre-trained NNJMs available with the generic models for fr-&gt;en and en-&gt;fr.
 4.0: fine-tune the generic NNJM or train your own for best hybrid neural-statistical MT results.</t>
+  </si>
+  <si>
+    <t>3.0: n/a
+4.0: incrAddSentence()</t>
+  </si>
+  <si>
+    <t>3.0: n/a
+4.0: incrStatus()</t>
+  </si>
+  <si>
+    <t>3.0: getVersion() exists and returns "PortageII-3.0"; WSDL says PortageII 3.0 (2016)
+4.0: getVersion() exists and returns "PortageII-4.0"; WSDL says PortageII 4.0 (2018)</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII API from PortageII 1.0 to PortageII 4.0</t>
+  </si>
+  <si>
+    <t>Evolution of the PortageII API from PortageII 1.0 to PortageII 4.0 (p. 2)</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1288,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1302,7 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="4" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1319,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>2</v>
@@ -1339,13 +1342,13 @@
         <v>17</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>34</v>
@@ -1359,7 +1362,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>6</v>
@@ -1415,14 +1418,14 @@
         <v>20</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D8" s="52"/>
       <c r="E8" s="50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F8" s="51"/>
     </row>
@@ -1431,7 +1434,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9" s="53" t="s">
         <v>21</v>
@@ -1465,7 +1468,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1485,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>2</v>
@@ -1568,13 +1571,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>36</v>
@@ -1582,19 +1585,19 @@
     </row>
     <row r="18" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="33" t="s">
         <v>73</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="F18" s="34" t="s">
         <v>25</v>
@@ -1602,33 +1605,33 @@
     </row>
     <row r="19" spans="1:6" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B19" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="E19" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>80</v>
-      </c>
       <c r="F19" s="34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D20" s="35" t="s">
         <v>25</v>
@@ -1642,10 +1645,10 @@
     </row>
     <row r="21" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>25</v>
@@ -1662,10 +1665,10 @@
     </row>
     <row r="22" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>25</v>
@@ -1691,7 +1694,7 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1708,61 +1711,61 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D26" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
     </row>
     <row r="27" spans="1:6" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="23" t="s">
-        <v>56</v>
-      </c>
       <c r="C27" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
     </row>
     <row r="28" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>25</v>
@@ -1772,16 +1775,16 @@
     </row>
     <row r="30" spans="1:6" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="6"/>
@@ -1789,7 +1792,7 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1806,58 +1809,58 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D33" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6"/>
     </row>
     <row r="35" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" s="33" t="s">
         <v>25</v>
@@ -1870,13 +1873,13 @@
     </row>
     <row r="37" spans="1:6" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>25</v>
@@ -1887,7 +1890,7 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1907,39 +1910,39 @@
         <v>0</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C42" s="45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D42" s="45"/>
       <c r="E42" s="45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F42" s="46"/>
     </row>
     <row r="43" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C43" s="47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D43" s="47"/>
       <c r="E43" s="48" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F43" s="49"/>
     </row>
     <row r="44" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C44" s="43" t="s">
         <v>25</v>
@@ -1952,10 +1955,10 @@
     </row>
     <row r="45" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C45" s="43" t="s">
         <v>25</v>
@@ -1968,10 +1971,10 @@
     </row>
     <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C46" s="43" t="s">
         <v>25</v>
@@ -1984,13 +1987,13 @@
     </row>
     <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C47" s="43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D47" s="43"/>
       <c r="E47" s="43"/>
@@ -1998,29 +2001,29 @@
     </row>
     <row r="48" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B48" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="43" t="s">
         <v>107</v>
-      </c>
-      <c r="C48" s="43" t="s">
-        <v>109</v>
       </c>
       <c r="D48" s="43"/>
       <c r="E48" s="43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F48" s="44"/>
     </row>
     <row r="49" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C49" s="63" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D49" s="63"/>
       <c r="E49" s="63"/>
@@ -2029,7 +2032,7 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
       <c r="B50" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2049,23 +2052,23 @@
         <v>0</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D52" s="45"/>
       <c r="E52" s="45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F52" s="46"/>
     </row>
     <row r="53" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B53" s="42" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C53" s="60" t="s">
         <v>25</v>
@@ -2078,13 +2081,13 @@
     </row>
     <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C54" s="43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D54" s="43"/>
       <c r="E54" s="43" t="s">
@@ -2094,26 +2097,26 @@
     </row>
     <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C55" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D55" s="65"/>
       <c r="E55" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F55" s="66"/>
     </row>
     <row r="56" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" s="52" t="s">
         <v>102</v>
-      </c>
-      <c r="B56" s="52" t="s">
-        <v>104</v>
       </c>
       <c r="C56" s="56"/>
       <c r="D56" s="56"/>
@@ -2122,13 +2125,13 @@
     </row>
     <row r="57" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C57" s="58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D57" s="58"/>
       <c r="E57" s="58"/>

</xml_diff>

<commit_message>
PortageAPIComparison.xlsx update from discussion yesterday: +NNJM -CoarseLM
</commit_message>
<xml_diff>
--- a/doc/PortageAPIComparison.xlsx
+++ b/doc/PortageAPIComparison.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="131">
   <si>
     <t>Task</t>
   </si>
@@ -213,9 +213,6 @@
   </si>
   <si>
     <t>Coarse LMs</t>
-  </si>
-  <si>
-    <t>Enable Coarse LMs with 200 and 800 classes (this new features is enabled by default)</t>
   </si>
   <si>
     <t>PortageII 2.2, 2.1 and 2.0 framework</t>
@@ -314,10 +311,6 @@
     <t>Loop over the above procedure, 10 sentences or paragraphs at a time. Avoid submitting sentences one at a time if you can, to amortize the fixed overhead over larger blocks instead.</t>
   </si>
   <si>
-    <t>This process reduces the size of your phrase tables.
-Only use it for very large, low quality corpora, with 10s of millions or sentence pairs or more.</t>
-  </si>
-  <si>
     <t>This  baseline reordering model is always required, and should always be used, preferably in combination with the new, sparse one.</t>
   </si>
   <si>
@@ -394,15 +387,7 @@
     <t>PortageII 3.0 and 4.0 framework</t>
   </si>
   <si>
-    <t>3.0: Yes. 3.0 includes important new features and many updates to the recommended training parameters: retrain all models from previous versions.
-4.0: retraining is required to train or fine tune your own NNJM, and to enable incremental document adaptation.</t>
-  </si>
-  <si>
     <t>NNJM</t>
-  </si>
-  <si>
-    <t>3.0: pre-trained NNJMs available with the generic models for fr-&gt;en and en-&gt;fr.
-4.0: fine-tune the generic NNJM or train your own for best hybrid neural-statistical MT results.</t>
   </si>
   <si>
     <t>3.0: n/a
@@ -421,6 +406,26 @@
   </si>
   <si>
     <t>Evolution of the PortageII API from PortageII 1.0 to PortageII 4.0 (p. 2)</t>
+  </si>
+  <si>
+    <t>3.0: Enable Coarse LMs with 200 and 800 classes (this new features is enabled by default)
+4.0: Use only if you don't fine-tune the generic NNJM or create your own NNJM.</t>
+  </si>
+  <si>
+    <t>This process reduces the size of your phrase tables.
+Only use it for very large corpora, with 10M sentence pairs or more.</t>
+  </si>
+  <si>
+    <t>same as 3.0/4.0</t>
+  </si>
+  <si>
+    <t>3.0: Yes. 3.0 includes important new features and many updates to the recommended training parameters: retrain all models from previous versions.
+4.0: Recommended. Retraining is required to train or fine tune your own NNJM, and to enable incremental document adaptation.
+However, 3.0 and 4.0 can still run older models.</t>
+  </si>
+  <si>
+    <t>3.0: pre-trained NNJMs available with the generic models for fr-&gt;en and en-&gt;fr.
+4.0: with small to medium corpora, we recommend you fine-tune the generic NNJM; with large corpora (2M sentence pairs or more), we recommend you train your own for best hybrid neural-statistical MT results. Requires a GPU; if you don't have one, use the pre-trained NNJMs, or Coarse LMs.</t>
   </si>
 </sst>
 </file>
@@ -912,18 +917,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -932,57 +988,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1287,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,7 +1307,7 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1322,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>2</v>
@@ -1342,7 +1347,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>5</v>
@@ -1362,7 +1367,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>6</v>
@@ -1404,14 +1409,14 @@
       <c r="B7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="50" t="s">
+      <c r="D7" s="48"/>
+      <c r="E7" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="51"/>
+      <c r="F7" s="60"/>
     </row>
     <row r="8" spans="1:6" ht="138" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
@@ -1420,30 +1425,30 @@
       <c r="B8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="50" t="s">
+      <c r="C8" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="51"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="60"/>
     </row>
     <row r="9" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="53" t="s">
+      <c r="D9" s="62"/>
+      <c r="E9" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="55"/>
+      <c r="F9" s="63"/>
     </row>
     <row r="10" spans="1:6" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="30" t="s">
@@ -1468,7 +1473,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1488,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>2</v>
@@ -1585,19 +1590,19 @@
     </row>
     <row r="18" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="C18" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="33" t="s">
         <v>72</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>73</v>
       </c>
       <c r="F18" s="34" t="s">
         <v>25</v>
@@ -1605,33 +1610,33 @@
     </row>
     <row r="19" spans="1:6" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B19" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="D19" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="E19" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="33" t="s">
-        <v>78</v>
-      </c>
       <c r="F19" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D20" s="35" t="s">
         <v>25</v>
@@ -1645,10 +1650,10 @@
     </row>
     <row r="21" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>25</v>
@@ -1665,10 +1670,10 @@
     </row>
     <row r="22" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>25</v>
@@ -1694,7 +1699,7 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1714,7 +1719,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>39</v>
@@ -1743,7 +1748,7 @@
     </row>
     <row r="28" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>58</v>
@@ -1752,14 +1757,14 @@
         <v>41</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>40</v>
@@ -1775,7 +1780,7 @@
     </row>
     <row r="30" spans="1:6" ht="134.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>49</v>
@@ -1792,7 +1797,7 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1812,7 +1817,7 @@
         <v>38</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>39</v>
@@ -1825,7 +1830,7 @@
     </row>
     <row r="34" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>51</v>
@@ -1834,33 +1839,33 @@
         <v>50</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6"/>
     </row>
     <row r="35" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="6"/>
     </row>
     <row r="36" spans="1:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C36" s="33" t="s">
         <v>25</v>
@@ -1873,13 +1878,13 @@
     </row>
     <row r="37" spans="1:6" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D37" s="26" t="s">
         <v>25</v>
@@ -1890,7 +1895,7 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1910,129 +1915,129 @@
         <v>0</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="F42" s="46"/>
-    </row>
-    <row r="43" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F42" s="58"/>
+    </row>
+    <row r="43" spans="1:6" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>60</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="C43" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="47"/>
-      <c r="E43" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="F43" s="49"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="66"/>
     </row>
     <row r="44" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="44"/>
-    </row>
-    <row r="45" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="C44" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="54"/>
+    </row>
+    <row r="45" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
         <v>64</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" s="44"/>
+        <v>126</v>
+      </c>
+      <c r="C45" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="54"/>
     </row>
     <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" s="44"/>
+        <v>69</v>
+      </c>
+      <c r="C46" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="54"/>
     </row>
     <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
         <v>62</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="44"/>
+        <v>104</v>
+      </c>
+      <c r="C47" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="54"/>
     </row>
     <row r="48" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
         <v>63</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="F48" s="44"/>
+        <v>103</v>
+      </c>
+      <c r="C48" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" s="53"/>
+      <c r="E48" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" s="54"/>
     </row>
     <row r="49" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="63" t="s">
-        <v>101</v>
-      </c>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="64"/>
+        <v>95</v>
+      </c>
+      <c r="C49" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="56"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
       <c r="B50" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2052,90 +2057,90 @@
         <v>0</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="57"/>
+      <c r="E52" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="F52" s="46"/>
-    </row>
-    <row r="53" spans="1:6" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F52" s="58"/>
+    </row>
+    <row r="53" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B53" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="C53" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="D53" s="61"/>
-      <c r="E53" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="F53" s="62"/>
+        <v>130</v>
+      </c>
+      <c r="C53" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" s="44"/>
+      <c r="E53" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="45"/>
     </row>
     <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B54" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="C54" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="D54" s="43"/>
-      <c r="E54" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F54" s="44"/>
+        <v>127</v>
+      </c>
+      <c r="C54" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="54"/>
     </row>
     <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="D55" s="65"/>
-      <c r="E55" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="F55" s="66"/>
+        <v>97</v>
+      </c>
+      <c r="C55" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D55" s="53"/>
+      <c r="E55" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" s="47"/>
     </row>
     <row r="56" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="52" t="s">
-        <v>102</v>
-      </c>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="57"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="50"/>
     </row>
     <row r="57" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="59"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="51"/>
+      <c r="F57" s="52"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="22"/>
@@ -2187,26 +2192,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C47:F47"/>
@@ -2217,6 +2202,26 @@
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="E44:F44"/>
     <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="B56:F56"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Generate updated PortageAPIComparison.pdf from PortageAPIComparison.xlsx
</commit_message>
<xml_diff>
--- a/doc/PortageAPIComparison.xlsx
+++ b/doc/PortageAPIComparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="30" windowWidth="13965" windowHeight="8475"/>
+    <workbookView xWindow="192" yWindow="36" windowWidth="13968" windowHeight="8472"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -917,6 +917,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -932,61 +983,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1292,19 +1292,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.28515625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="23.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" style="1" customWidth="1"/>
+    <col min="3" max="5" width="23.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="4" t="s">
         <v>124</v>
@@ -1409,14 +1409,14 @@
       <c r="B7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="59" t="s">
+      <c r="D7" s="52"/>
+      <c r="E7" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="60"/>
+      <c r="F7" s="51"/>
     </row>
     <row r="8" spans="1:6" ht="138" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
@@ -1425,14 +1425,14 @@
       <c r="B8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="59" t="s">
+      <c r="D8" s="52"/>
+      <c r="E8" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="60"/>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
@@ -1441,14 +1441,14 @@
       <c r="B9" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="62"/>
-      <c r="E9" s="61" t="s">
+      <c r="D9" s="54"/>
+      <c r="E9" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="63"/>
+      <c r="F9" s="55"/>
     </row>
     <row r="10" spans="1:6" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="30" t="s">
@@ -1470,7 +1470,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>125</v>
@@ -1688,7 +1688,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1696,7 +1696,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="4" t="s">
         <v>116</v>
@@ -1794,7 +1794,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
         <v>114</v>
@@ -1892,7 +1892,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
       <c r="B40" s="4" t="s">
         <v>117</v>
@@ -1917,30 +1917,30 @@
       <c r="B42" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="57" t="s">
+      <c r="C42" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57" t="s">
+      <c r="D42" s="45"/>
+      <c r="E42" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="F42" s="58"/>
-    </row>
-    <row r="43" spans="1:6" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F42" s="46"/>
+    </row>
+    <row r="43" spans="1:6" ht="113.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>60</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="64" t="s">
+      <c r="C43" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="64"/>
-      <c r="E43" s="65" t="s">
+      <c r="D43" s="47"/>
+      <c r="E43" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="F43" s="66"/>
+      <c r="F43" s="49"/>
     </row>
     <row r="44" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
@@ -1949,14 +1949,14 @@
       <c r="B44" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="54"/>
+      <c r="C44" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="44"/>
     </row>
     <row r="45" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
@@ -1965,14 +1965,14 @@
       <c r="B45" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" s="54"/>
+      <c r="C45" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="44"/>
     </row>
     <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
@@ -1981,14 +1981,14 @@
       <c r="B46" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" s="54"/>
+      <c r="C46" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="44"/>
     </row>
     <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
@@ -1997,12 +1997,12 @@
       <c r="B47" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="53" t="s">
+      <c r="C47" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="54"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="44"/>
     </row>
     <row r="48" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
@@ -2011,14 +2011,14 @@
       <c r="B48" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="53" t="s">
+      <c r="C48" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D48" s="53"/>
-      <c r="E48" s="53" t="s">
+      <c r="D48" s="43"/>
+      <c r="E48" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="F48" s="54"/>
+      <c r="F48" s="44"/>
     </row>
     <row r="49" spans="1:6" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="30" t="s">
@@ -2027,14 +2027,14 @@
       <c r="B49" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="55" t="s">
+      <c r="C49" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="56"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="59"/>
+    </row>
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
       <c r="B50" s="4" t="s">
         <v>118</v>
@@ -2059,14 +2059,14 @@
       <c r="B52" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C52" s="57" t="s">
+      <c r="C52" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57" t="s">
+      <c r="D52" s="45"/>
+      <c r="E52" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="F52" s="58"/>
+      <c r="F52" s="46"/>
     </row>
     <row r="53" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
@@ -2075,14 +2075,14 @@
       <c r="B53" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="C53" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="D53" s="44"/>
-      <c r="E53" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F53" s="45"/>
+      <c r="C53" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" s="61"/>
+      <c r="E53" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="62"/>
     </row>
     <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
@@ -2091,14 +2091,14 @@
       <c r="B54" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="C54" s="53" t="s">
+      <c r="C54" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D54" s="53"/>
-      <c r="E54" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="F54" s="54"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="44"/>
     </row>
     <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
@@ -2107,26 +2107,26 @@
       <c r="B55" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="53" t="s">
+      <c r="C55" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="53"/>
-      <c r="E55" s="46" t="s">
+      <c r="D55" s="43"/>
+      <c r="E55" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="F55" s="47"/>
+      <c r="F55" s="64"/>
     </row>
     <row r="56" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B56" s="48" t="s">
+      <c r="B56" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="50"/>
+      <c r="C56" s="65"/>
+      <c r="D56" s="65"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="66"/>
     </row>
     <row r="57" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="30" t="s">
@@ -2135,14 +2135,14 @@
       <c r="B57" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="51" t="s">
+      <c r="C57" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="51"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="52"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="57"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="22"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2150,7 +2150,7 @@
       <c r="E58" s="5"/>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="22"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2158,7 +2158,7 @@
       <c r="E59" s="5"/>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="22"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2166,7 +2166,7 @@
       <c r="E60" s="5"/>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="22"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -2174,7 +2174,7 @@
       <c r="E61" s="5"/>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="22"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -2182,7 +2182,7 @@
       <c r="E62" s="5"/>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="22"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2192,22 +2192,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
     <mergeCell ref="C57:F57"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="C54:D54"/>
@@ -2222,6 +2206,22 @@
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="E55:F55"/>
     <mergeCell ref="B56:F56"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -2241,7 +2241,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2253,7 +2253,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>